<commit_message>
Creatinn new branch develop
</commit_message>
<xml_diff>
--- a/Avance.xlsx
+++ b/Avance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://innovaccion-my.sharepoint.com/personal/lx14702_innovaccion_mx/Documents/4.Java/FullStackJavaTecsup/BootcampJava/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="119" documentId="13_ncr:1_{6E3EBEFD-7FD4-4C45-91E3-C9FB228A1C6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C29121D4-159F-7F40-B6BF-D19D902DD6E5}"/>
+  <xr:revisionPtr revIDLastSave="131" documentId="13_ncr:1_{6E3EBEFD-7FD4-4C45-91E3-C9FB228A1C6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0B903801-52C7-7943-A4FB-0FC39006B2D6}"/>
   <bookViews>
-    <workbookView xWindow="2940" yWindow="2820" windowWidth="23300" windowHeight="13260" xr2:uid="{9B8E8FEF-6B14-ED49-B192-ACDD11EA36C9}"/>
+    <workbookView xWindow="1700" yWindow="1400" windowWidth="23300" windowHeight="13260" xr2:uid="{9B8E8FEF-6B14-ED49-B192-ACDD11EA36C9}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="111">
   <si>
     <t>https://tecsup.webex.com/tecsup/ldr.php?RCID=9f4869bf786c0f70b91301fdb76e9763</t>
   </si>
@@ -348,6 +348,27 @@
   </si>
   <si>
     <t>Tests y Security</t>
+  </si>
+  <si>
+    <t>https://tecsup.webex.com/tecsup/ldr.php?RCID=0acab4db96997e9e9900eb9c64487d02</t>
+  </si>
+  <si>
+    <t>8Tu4v6PB</t>
+  </si>
+  <si>
+    <t>https://tecsup.webex.com/tecsup/ldr.php?RCID=f5df756e0325ba56b6b9cf08c928505b</t>
+  </si>
+  <si>
+    <t>pK5X2sHM</t>
+  </si>
+  <si>
+    <t>https://tecsup.webex.com/tecsup/ldr.php?RCID=5548264b82c24dc9378bd22623e95c9a</t>
+  </si>
+  <si>
+    <t>iMmwWu8x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ramas de GIT, </t>
   </si>
 </sst>
 </file>
@@ -741,10 +762,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A61CE00-3EAC-F24D-BCD8-995A8148363B}">
-  <dimension ref="A2:F46"/>
+  <dimension ref="A2:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="E41" sqref="E41"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1279,6 +1300,45 @@
       </c>
       <c r="E46" t="s">
         <v>101</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47" s="1">
+        <v>45420</v>
+      </c>
+      <c r="C47" t="s">
+        <v>110</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="E47" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48" s="1">
+        <v>45421</v>
+      </c>
+      <c r="C48" t="s">
+        <v>46</v>
+      </c>
+      <c r="D48" t="s">
+        <v>106</v>
+      </c>
+      <c r="E48" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A49" s="1">
+        <v>45422</v>
+      </c>
+      <c r="D49" t="s">
+        <v>108</v>
+      </c>
+      <c r="E49" t="s">
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -1311,6 +1371,7 @@
     <hyperlink ref="E44" r:id="rId26" display="https://tecsup.webex.com/tecsup/ldr.php?RCID=338761822c86e6791e90ffd3a3877c26" xr:uid="{2DD6AECD-E770-F147-B385-C10B0A78C7D7}"/>
     <hyperlink ref="D43" r:id="rId27" xr:uid="{DD6B0C72-2FB5-8E40-94BF-1BE2194E1A8F}"/>
     <hyperlink ref="D42" r:id="rId28" xr:uid="{40A6377A-AA5A-0548-B6FF-668203D83EE8}"/>
+    <hyperlink ref="D47" r:id="rId29" xr:uid="{D245833C-4286-3140-8C71-16C42E4BD97F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>